<commit_message>
sql script to make the DB
</commit_message>
<xml_diff>
--- a/template/covid_wwtp_data_template.xlsx
+++ b/template/covid_wwtp_data_template.xlsx
@@ -1101,6 +1101,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002CEA048A63282C439189779433474EBB" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="30a104bdd4c4acb56935c0dc758ef385">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="41e6d880-c95d-428b-b867-28a86f690840" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d83beaf89990ec78dc26f849fcf6fbe8" ns2:_="">
     <xsd:import namespace="41e6d880-c95d-428b-b867-28a86f690840"/>
@@ -1232,22 +1247,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C78F5240-8910-4EAB-A5A8-13C69138C2A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="41e6d880-c95d-428b-b867-28a86f690840"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D8F596A-8119-441E-8E72-3B8F82046F19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE1836F9-99A6-4424-A180-C73D29D93311}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1263,28 +1287,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D8F596A-8119-441E-8E72-3B8F82046F19}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C78F5240-8910-4EAB-A5A8-13C69138C2A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="41e6d880-c95d-428b-b867-28a86f690840"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>